<commit_message>
UPDATE data for Washington, D.C.
</commit_message>
<xml_diff>
--- a/source_code/data/ates.xlsx
+++ b/source_code/data/ates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\district_thermal_energy_systems_with_power_markets\source_code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B60A44-A4A1-4148-8DF2-446FA21D794F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DABAEF-47F3-4E5F-804C-AA2AF808523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30840" yWindow="2280" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3000</v>
+        <v>3300.0000000000005</v>
       </c>
       <c r="F2">
         <v>0.01</v>
@@ -437,7 +437,7 @@
         <v>7.2629999999999999</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -493,7 +493,8 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3000</v>
+        <f>'2025'!E2*(1-0.25*0.2)</f>
+        <v>3135.0000000000005</v>
       </c>
       <c r="F2">
         <v>0.01</v>
@@ -502,7 +503,7 @@
         <v>7.2629999999999999</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -558,7 +559,8 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3000</v>
+        <f>'2025'!E2*(1-0.25*0.4)</f>
+        <v>2970.0000000000005</v>
       </c>
       <c r="F2">
         <v>0.01</v>
@@ -567,7 +569,7 @@
         <v>7.2629999999999999</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +625,8 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3000</v>
+        <f>'2025'!E2*(1-0.25*0.6)</f>
+        <v>2805.0000000000005</v>
       </c>
       <c r="F2">
         <v>0.01</v>
@@ -632,7 +635,7 @@
         <v>7.2629999999999999</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +691,8 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3000</v>
+        <f>'2025'!E2*(1-0.25*0.8)</f>
+        <v>2640.0000000000005</v>
       </c>
       <c r="F2">
         <v>0.01</v>
@@ -697,7 +701,7 @@
         <v>7.2629999999999999</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -753,7 +757,8 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>3000</v>
+        <f>'2025'!E2*(1-0.25*1)</f>
+        <v>2475.0000000000005</v>
       </c>
       <c r="F2">
         <v>0.01</v>
@@ -762,7 +767,7 @@
         <v>7.2629999999999999</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>